<commit_message>
Updated Documents for Release
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/ProductBurndown.xlsx
+++ b/01_ProjectPlanning/ProductBurndown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Schule\SYP\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Dropbox\Schule\SYP\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -510,49 +510,49 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>24.3</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>21.6</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>21.6</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>18.900000000000002</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>17.400000000000002</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>15.900000000000002</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>13.200000000000003</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>10.500000000000004</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>7.8000000000000043</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.100000000000005</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.9500000000000051</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1042,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2389,8 +2389,12 @@
         <v>18</v>
       </c>
       <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+      <c r="E38" s="6">
+        <v>18</v>
+      </c>
       <c r="F38" s="7">
         <f t="shared" si="5"/>
         <v>27</v>
@@ -2409,11 +2413,11 @@
       </c>
       <c r="J38" s="7">
         <f t="shared" si="3"/>
-        <v>24.3</v>
+        <v>27</v>
       </c>
       <c r="K38" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2425,11 +2429,15 @@
         <v>18</v>
       </c>
       <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+      <c r="D39" s="6">
+        <v>0</v>
+      </c>
+      <c r="E39" s="6">
+        <v>18</v>
+      </c>
       <c r="F39" s="7">
         <f t="shared" si="5"/>
-        <v>24.3</v>
+        <v>27</v>
       </c>
       <c r="G39" s="7">
         <f t="shared" si="6"/>
@@ -2441,15 +2449,15 @@
       </c>
       <c r="I39" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>378</v>
       </c>
       <c r="J39" s="7">
         <f t="shared" si="3"/>
-        <v>21.6</v>
+        <v>27</v>
       </c>
       <c r="K39" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.13636363636363635</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2461,11 +2469,15 @@
         <v>0</v>
       </c>
       <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="D40" s="6">
+        <v>0</v>
+      </c>
+      <c r="E40" s="6">
+        <v>0</v>
+      </c>
       <c r="F40" s="7">
         <f t="shared" si="5"/>
-        <v>21.6</v>
+        <v>27</v>
       </c>
       <c r="G40" s="7">
         <f t="shared" si="6"/>
@@ -2477,15 +2489,15 @@
       </c>
       <c r="I40" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>396</v>
       </c>
       <c r="J40" s="7">
         <f t="shared" si="3"/>
-        <v>21.6</v>
+        <v>27</v>
       </c>
       <c r="K40" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.13636363636363635</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2497,11 +2509,15 @@
         <v>18</v>
       </c>
       <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+      <c r="D41" s="6">
+        <v>0</v>
+      </c>
+      <c r="E41" s="6">
+        <v>12</v>
+      </c>
       <c r="F41" s="7">
         <f t="shared" si="5"/>
-        <v>21.6</v>
+        <v>27</v>
       </c>
       <c r="G41" s="7">
         <f t="shared" si="6"/>
@@ -2513,15 +2529,15 @@
       </c>
       <c r="I41" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>396</v>
       </c>
       <c r="J41" s="7">
         <f t="shared" si="3"/>
-        <v>18.900000000000002</v>
+        <v>27</v>
       </c>
       <c r="K41" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.13235294117647059</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2533,11 +2549,15 @@
         <v>10</v>
       </c>
       <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+      <c r="D42" s="6">
+        <v>0</v>
+      </c>
+      <c r="E42" s="6">
+        <v>0</v>
+      </c>
       <c r="F42" s="7">
         <f t="shared" si="5"/>
-        <v>18.900000000000002</v>
+        <v>27</v>
       </c>
       <c r="G42" s="7">
         <f t="shared" si="6"/>
@@ -2549,15 +2569,15 @@
       </c>
       <c r="I42" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>408</v>
       </c>
       <c r="J42" s="7">
         <f t="shared" si="3"/>
-        <v>17.400000000000002</v>
+        <v>27</v>
       </c>
       <c r="K42" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.13235294117647059</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2569,11 +2589,15 @@
         <v>10</v>
       </c>
       <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+      <c r="D43" s="6">
+        <v>0</v>
+      </c>
+      <c r="E43" s="6">
+        <v>0</v>
+      </c>
       <c r="F43" s="7">
         <f t="shared" si="5"/>
-        <v>17.400000000000002</v>
+        <v>27</v>
       </c>
       <c r="G43" s="7">
         <f t="shared" si="6"/>
@@ -2585,15 +2609,15 @@
       </c>
       <c r="I43" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>408</v>
       </c>
       <c r="J43" s="7">
         <f t="shared" si="3"/>
-        <v>15.900000000000002</v>
+        <v>27</v>
       </c>
       <c r="K43" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.13235294117647059</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2605,11 +2629,15 @@
         <v>18</v>
       </c>
       <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+      <c r="D44" s="6">
+        <v>0</v>
+      </c>
+      <c r="E44" s="6">
+        <v>12</v>
+      </c>
       <c r="F44" s="7">
         <f t="shared" si="5"/>
-        <v>15.900000000000002</v>
+        <v>27</v>
       </c>
       <c r="G44" s="7">
         <f t="shared" si="6"/>
@@ -2621,15 +2649,15 @@
       </c>
       <c r="I44" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>408</v>
       </c>
       <c r="J44" s="7">
         <f t="shared" si="3"/>
-        <v>13.200000000000003</v>
+        <v>27</v>
       </c>
       <c r="K44" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.12857142857142856</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -2641,11 +2669,15 @@
         <v>18</v>
       </c>
       <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
+      <c r="D45" s="6">
+        <v>0</v>
+      </c>
+      <c r="E45" s="6">
+        <v>18</v>
+      </c>
       <c r="F45" s="7">
         <f t="shared" si="5"/>
-        <v>13.200000000000003</v>
+        <v>27</v>
       </c>
       <c r="G45" s="7">
         <f t="shared" si="6"/>
@@ -2657,15 +2689,15 @@
       </c>
       <c r="I45" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="J45" s="7">
         <f t="shared" si="3"/>
-        <v>10.500000000000004</v>
+        <v>27</v>
       </c>
       <c r="K45" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.12328767123287671</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -2677,11 +2709,15 @@
         <v>18</v>
       </c>
       <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
+      <c r="D46" s="6">
+        <v>0</v>
+      </c>
+      <c r="E46" s="6">
+        <v>18</v>
+      </c>
       <c r="F46" s="7">
         <f t="shared" si="5"/>
-        <v>10.500000000000004</v>
+        <v>27</v>
       </c>
       <c r="G46" s="7">
         <f t="shared" si="6"/>
@@ -2693,15 +2729,15 @@
       </c>
       <c r="I46" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="J46" s="7">
         <f t="shared" si="3"/>
-        <v>7.8000000000000043</v>
+        <v>27</v>
       </c>
       <c r="K46" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.11842105263157894</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -2713,11 +2749,15 @@
         <v>18</v>
       </c>
       <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
+      <c r="D47" s="6">
+        <v>0</v>
+      </c>
+      <c r="E47" s="6">
+        <v>18</v>
+      </c>
       <c r="F47" s="7">
         <f t="shared" si="5"/>
-        <v>7.8000000000000043</v>
+        <v>27</v>
       </c>
       <c r="G47" s="7">
         <f t="shared" si="6"/>
@@ -2729,15 +2769,15 @@
       </c>
       <c r="I47" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>456</v>
       </c>
       <c r="J47" s="7">
         <f t="shared" si="3"/>
-        <v>5.100000000000005</v>
+        <v>27</v>
       </c>
       <c r="K47" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.11392405063291139</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2749,11 +2789,15 @@
         <v>21</v>
       </c>
       <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+      <c r="D48" s="6">
+        <v>0</v>
+      </c>
+      <c r="E48" s="6">
+        <v>2</v>
+      </c>
       <c r="F48" s="7">
         <f t="shared" si="5"/>
-        <v>5.100000000000005</v>
+        <v>27</v>
       </c>
       <c r="G48" s="7">
         <f t="shared" si="6"/>
@@ -2765,15 +2809,15 @@
       </c>
       <c r="I48" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>474</v>
       </c>
       <c r="J48" s="7">
         <f t="shared" si="3"/>
-        <v>1.9500000000000051</v>
+        <v>27</v>
       </c>
       <c r="K48" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.1134453781512605</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -2785,11 +2829,15 @@
         <v>21</v>
       </c>
       <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
+      <c r="D49" s="6">
+        <v>0</v>
+      </c>
+      <c r="E49" s="6">
+        <v>3</v>
+      </c>
       <c r="F49" s="7">
         <f t="shared" si="5"/>
-        <v>1.9500000000000051</v>
+        <v>27</v>
       </c>
       <c r="G49" s="7">
         <f t="shared" si="6"/>
@@ -2801,15 +2849,15 @@
       </c>
       <c r="I49" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>476</v>
       </c>
       <c r="J49" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="K49" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.11273486430062631</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -2821,11 +2869,15 @@
         <v>21</v>
       </c>
       <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+      <c r="D50" s="6">
+        <v>0</v>
+      </c>
+      <c r="E50" s="6">
+        <v>0</v>
+      </c>
       <c r="F50" s="7">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G50" s="7">
         <f t="shared" si="6"/>
@@ -2837,15 +2889,15 @@
       </c>
       <c r="I50" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>479</v>
       </c>
       <c r="J50" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="K50" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.11273486430062631</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -2857,11 +2909,15 @@
         <v>21</v>
       </c>
       <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
+      <c r="D51" s="6">
+        <v>3</v>
+      </c>
+      <c r="E51" s="6">
+        <v>18</v>
+      </c>
       <c r="F51" s="7">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G51" s="7">
         <f t="shared" si="6"/>
@@ -2869,19 +2925,19 @@
       </c>
       <c r="H51" s="7">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I51" s="7">
         <f t="shared" si="2"/>
-        <v>360</v>
+        <v>479</v>
       </c>
       <c r="J51" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="K51" s="9">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>0.11468812877263582</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2893,36 +2949,40 @@
         <v>21</v>
       </c>
       <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
+      <c r="D52" s="6">
+        <v>1</v>
+      </c>
+      <c r="E52" s="6">
+        <v>18</v>
+      </c>
       <c r="F52" s="7">
         <f>J51+C52</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G52" s="7">
         <f>H51</f>
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H52" s="7">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I52" s="7">
         <f>I51+E51</f>
-        <v>360</v>
+        <v>497</v>
       </c>
       <c r="J52" s="7">
         <f>MAX(IF(OR(ISBLANK(D52),ISBLANK(E52)),F52-K51*B52,F52-D52),0)</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K52" s="9">
         <f>IF(OR(ISBLANK(D52),ISBLANK(E52)),K51,H52/(I52+E52))</f>
-        <v>0.15</v>
+        <v>0.11262135922330097</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
-        <f t="shared" ref="A53:A55" si="7">A52+7</f>
+        <f t="shared" ref="A53:A58" si="7">A52+7</f>
         <v>43174</v>
       </c>
       <c r="B53" s="6">
@@ -2930,30 +2990,32 @@
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
+      <c r="E53" s="6">
+        <v>18</v>
+      </c>
       <c r="F53" s="7">
         <f t="shared" ref="F53:F55" si="8">J52+C53</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G53" s="7">
         <f t="shared" ref="G53:G55" si="9">H52</f>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H53" s="7">
         <f t="shared" ref="H53:H55" si="10">G53+D53</f>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I53" s="7">
         <f t="shared" ref="I53:I55" si="11">I52+E52</f>
-        <v>360</v>
+        <v>515</v>
       </c>
       <c r="J53" s="7">
         <f t="shared" ref="J53:J55" si="12">MAX(IF(OR(ISBLANK(D53),ISBLANK(E53)),F53-K52*B53,F53-D53),0)</f>
-        <v>0</v>
+        <v>20.634951456310681</v>
       </c>
       <c r="K53" s="9">
         <f t="shared" ref="K53:K55" si="13">IF(OR(ISBLANK(D53),ISBLANK(E53)),K52,H53/(I53+E53))</f>
-        <v>0.15</v>
+        <v>0.11262135922330097</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2966,30 +3028,32 @@
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
+      <c r="E54" s="6">
+        <v>18</v>
+      </c>
       <c r="F54" s="7">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>20.634951456310681</v>
       </c>
       <c r="G54" s="7">
         <f t="shared" si="9"/>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H54" s="7">
         <f t="shared" si="10"/>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I54" s="7">
         <f t="shared" si="11"/>
-        <v>360</v>
+        <v>533</v>
       </c>
       <c r="J54" s="7">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>18.269902912621362</v>
       </c>
       <c r="K54" s="9">
         <f t="shared" si="13"/>
-        <v>0.15</v>
+        <v>0.11262135922330097</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -3002,53 +3066,167 @@
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
+      <c r="E55" s="6">
+        <v>12</v>
+      </c>
       <c r="F55" s="7">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>18.269902912621362</v>
       </c>
       <c r="G55" s="7">
         <f t="shared" si="9"/>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H55" s="7">
         <f t="shared" si="10"/>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I55" s="7">
         <f t="shared" si="11"/>
-        <v>360</v>
+        <v>551</v>
       </c>
       <c r="J55" s="7">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>15.904854368932043</v>
       </c>
       <c r="K55" s="9">
         <f t="shared" si="13"/>
-        <v>0.15</v>
+        <v>0.11262135922330097</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
-      <c r="B56" s="11">
+      <c r="A56" s="5">
+        <f t="shared" si="7"/>
+        <v>43195</v>
+      </c>
+      <c r="B56" s="6">
+        <v>22</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6">
+        <v>18</v>
+      </c>
+      <c r="F56" s="7">
+        <f t="shared" ref="F56:F57" si="14">J55+C56</f>
+        <v>15.904854368932043</v>
+      </c>
+      <c r="G56" s="7">
+        <f t="shared" ref="G56:G57" si="15">H55</f>
+        <v>58</v>
+      </c>
+      <c r="H56" s="7">
+        <f t="shared" ref="H56:H57" si="16">G56+D56</f>
+        <v>58</v>
+      </c>
+      <c r="I56" s="7">
+        <f t="shared" ref="I56:I57" si="17">I55+E55</f>
+        <v>563</v>
+      </c>
+      <c r="J56" s="7">
+        <f t="shared" ref="J56:J57" si="18">MAX(IF(OR(ISBLANK(D56),ISBLANK(E56)),F56-K55*B56,F56-D56),0)</f>
+        <v>13.427184466019421</v>
+      </c>
+      <c r="K56" s="9">
+        <f t="shared" ref="K56:K57" si="19">IF(OR(ISBLANK(D56),ISBLANK(E56)),K55,H56/(I56+E56))</f>
+        <v>0.11262135922330097</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <f t="shared" si="7"/>
+        <v>43202</v>
+      </c>
+      <c r="B57" s="6">
+        <v>23</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="7">
+        <f t="shared" si="14"/>
+        <v>13.427184466019421</v>
+      </c>
+      <c r="G57" s="7">
+        <f t="shared" si="15"/>
+        <v>58</v>
+      </c>
+      <c r="H57" s="7">
+        <f t="shared" si="16"/>
+        <v>58</v>
+      </c>
+      <c r="I57" s="7">
+        <f t="shared" si="17"/>
+        <v>581</v>
+      </c>
+      <c r="J57" s="7">
+        <f t="shared" si="18"/>
+        <v>10.836893203883498</v>
+      </c>
+      <c r="K57" s="9">
+        <f t="shared" si="19"/>
+        <v>0.11262135922330097</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <f t="shared" si="7"/>
+        <v>43209</v>
+      </c>
+      <c r="B58" s="6">
+        <v>24</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6">
+        <v>2</v>
+      </c>
+      <c r="F58" s="7">
+        <f t="shared" ref="F58" si="20">J57+C58</f>
+        <v>10.836893203883498</v>
+      </c>
+      <c r="G58" s="7">
+        <f t="shared" ref="G58" si="21">H57</f>
+        <v>58</v>
+      </c>
+      <c r="H58" s="7">
+        <f t="shared" ref="H58" si="22">G58+D58</f>
+        <v>58</v>
+      </c>
+      <c r="I58" s="7">
+        <f t="shared" ref="I58" si="23">I57+E57</f>
+        <v>581</v>
+      </c>
+      <c r="J58" s="7">
+        <f t="shared" ref="J58" si="24">MAX(IF(OR(ISBLANK(D58),ISBLANK(E58)),F58-K57*B58,F58-D58),0)</f>
+        <v>8.1339805825242752</v>
+      </c>
+      <c r="K58" s="9">
+        <f t="shared" ref="K58" si="25">IF(OR(ISBLANK(D58),ISBLANK(E58)),K57,H58/(I58+E58))</f>
+        <v>0.11262135922330097</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="10"/>
+      <c r="B59" s="11">
         <f>SUM(B7:B31)</f>
         <v>271</v>
       </c>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11">
+      <c r="C59" s="11"/>
+      <c r="D59" s="11">
         <f>AVERAGE(D7:D55)</f>
-        <v>1.7419354838709677</v>
-      </c>
-      <c r="E56" s="11">
-        <f>AVERAGE(E7:E55)</f>
-        <v>11.612903225806452</v>
-      </c>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="12"/>
+        <v>1.2608695652173914</v>
+      </c>
+      <c r="E59" s="11">
+        <f>AVERAGE(E7:E56)</f>
+        <v>11.62</v>
+      </c>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>